<commit_message>
Updated test and file to include columns with spaces
</commit_message>
<xml_diff>
--- a/tests/samples/empty_cols.xlsx
+++ b/tests/samples/empty_cols.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\15122\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7FDFC6B3-E16A-4628-B154-5910D1C32C4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05387D1B-6FC4-4882-AC22-6B9657C561E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Find</t>
   </si>
@@ -50,6 +63,21 @@
   </si>
   <si>
     <t>Empty2</t>
+  </si>
+  <si>
+    <t>Also Empty</t>
+  </si>
+  <si>
+    <t>Not Empty</t>
+  </si>
+  <si>
+    <t>This</t>
+  </si>
+  <si>
+    <t>is not</t>
+  </si>
+  <si>
+    <t>empty</t>
   </si>
 </sst>
 </file>
@@ -121,7 +149,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -426,15 +454,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -442,33 +470,48 @@
         <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated replace to be more aggressive and capture space only strings
</commit_message>
<xml_diff>
--- a/tests/samples/empty_cols.xlsx
+++ b/tests/samples/empty_cols.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\15122\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05387D1B-6FC4-4882-AC22-6B9657C561E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7B5696D-7380-47A3-8B5C-355852DF6376}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Find</t>
   </si>
@@ -62,9 +62,6 @@
     <t>Empty1</t>
   </si>
   <si>
-    <t>Empty2</t>
-  </si>
-  <si>
     <t>Also Empty</t>
   </si>
   <si>
@@ -78,6 +75,18 @@
   </si>
   <si>
     <t>empty</t>
+  </si>
+  <si>
+    <t>Spaces</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">         </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -457,7 +466,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -470,16 +479,16 @@
         <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -487,10 +496,13 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E2" t="s">
         <v>3</v>
+      </c>
+      <c r="F2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -498,10 +510,13 @@
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
         <v>5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -509,10 +524,13 @@
         <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E4" t="s">
         <v>7</v>
+      </c>
+      <c r="F4" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>